<commit_message>
Mejora en deseño y visualización
</commit_message>
<xml_diff>
--- a/Financiero - copia.xlsx
+++ b/Financiero - copia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Olimpia IT S.A.S\Descargas\gestor_proveedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gestor_proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505BAC88-2AEC-45F0-B8AC-D3FB97E0F753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0855CE65-0628-4509-B9FE-76C30CAF3A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proveedores" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="22">
   <si>
     <t>Id</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Compra</t>
-  </si>
-  <si>
-    <t>Ahorro</t>
   </si>
   <si>
     <t>Abono</t>
@@ -88,10 +85,10 @@
     <t>Total Facturas</t>
   </si>
   <si>
-    <t>Total Ahorro</t>
+    <t>Pepito</t>
   </si>
   <si>
-    <t>Pepito</t>
+    <t>Total Abonos</t>
   </si>
 </sst>
 </file>
@@ -299,7 +296,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Proveedor"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total Facturas" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Total Ahorro"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Total Abonos"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Saldo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -627,7 +624,7 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,7 +848,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
         <v>13828960</v>
@@ -871,7 +868,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3">
         <v>26554608</v>
@@ -891,7 +888,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
         <v>12050000</v>
@@ -911,7 +908,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3">
         <v>45000000</v>
@@ -931,7 +928,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3">
         <v>9000000</v>
@@ -951,7 +948,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
         <v>5994800</v>
@@ -971,7 +968,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" s="3">
         <v>5341300</v>
@@ -991,7 +988,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3">
         <v>18976000</v>
@@ -1011,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3">
         <v>10000000</v>
@@ -1031,7 +1028,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3">
         <v>10000000</v>
@@ -1051,7 +1048,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3">
         <v>10000000</v>
@@ -1071,7 +1068,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3">
         <v>20000000</v>
@@ -1091,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" s="3">
         <v>10000000</v>
@@ -1111,7 +1108,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="3">
         <v>4000000</v>
@@ -1131,7 +1128,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3">
         <v>18500000</v>
@@ -1151,7 +1148,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3">
         <v>10000000</v>
@@ -1171,7 +1168,7 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3">
         <v>10089200</v>
@@ -1191,7 +1188,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3">
         <v>16994000</v>
@@ -1211,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" s="3">
         <v>5500000</v>
@@ -1231,7 +1228,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" s="3">
         <v>6000000</v>
@@ -1251,7 +1248,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F31" s="3">
         <v>4000000</v>
@@ -1271,7 +1268,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3">
         <v>14064000</v>
@@ -1291,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33" s="3">
         <v>19450000</v>
@@ -1311,7 +1308,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" s="3">
         <v>22000000</v>
@@ -1331,7 +1328,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F35" s="3">
         <v>17000000</v>
@@ -1351,7 +1348,7 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3">
         <v>3000000</v>
@@ -1371,7 +1368,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" s="3">
         <v>3000000</v>
@@ -1391,7 +1388,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" s="3">
         <v>1480000</v>
@@ -1411,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" s="3">
         <v>2133000</v>
@@ -1431,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" s="3">
         <v>3000000</v>
@@ -1451,7 +1448,7 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F41" s="3">
         <v>80000</v>
@@ -1471,7 +1468,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F42" s="3">
         <v>64087000</v>
@@ -1491,7 +1488,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F43" s="3">
         <v>20000000</v>
@@ -1511,7 +1508,7 @@
         <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F44" s="3">
         <v>15700000</v>
@@ -1531,7 +1528,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45" s="3">
         <v>30000000</v>
@@ -1551,7 +1548,7 @@
         <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" s="3">
         <v>3680000</v>
@@ -1571,7 +1568,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F47" s="3">
         <v>42000000</v>
@@ -1591,7 +1588,7 @@
         <v>10</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F48" s="3">
         <v>17000000</v>
@@ -1611,7 +1608,7 @@
         <v>10</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F49" s="3">
         <v>12000000</v>
@@ -1631,7 +1628,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50" s="3">
         <v>8000000</v>
@@ -1651,7 +1648,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F51" s="3">
         <v>1300000</v>
@@ -1665,7 +1662,7 @@
         <v>45862</v>
       </c>
       <c r="C52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -1685,7 +1682,7 @@
         <v>45864</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -1705,7 +1702,7 @@
         <v>45865</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -1725,13 +1722,13 @@
         <v>45863</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D55" t="s">
         <v>10</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F55" s="3">
         <v>76190000</v>
@@ -1745,13 +1742,13 @@
         <v>45866</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D56" t="s">
         <v>10</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F56" s="3">
         <v>18448000</v>
@@ -1765,13 +1762,13 @@
         <v>45870</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57" s="3">
         <v>50000000</v>
@@ -1785,7 +1782,7 @@
         <v>45871</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -1805,7 +1802,7 @@
         <v>45871</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -1825,7 +1822,7 @@
         <v>45872</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -1845,7 +1842,7 @@
         <v>45828</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
@@ -1865,7 +1862,7 @@
         <v>45828</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -1885,7 +1882,7 @@
         <v>45832</v>
       </c>
       <c r="C63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -1905,7 +1902,7 @@
         <v>45832</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
@@ -1925,7 +1922,7 @@
         <v>45820</v>
       </c>
       <c r="C65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -1945,7 +1942,7 @@
         <v>45867</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -1965,7 +1962,7 @@
         <v>45867</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -1985,7 +1982,7 @@
         <v>45867</v>
       </c>
       <c r="C68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
@@ -2005,7 +2002,7 @@
         <v>45867</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -2025,7 +2022,7 @@
         <v>45867</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -2045,13 +2042,13 @@
         <v>45827</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D71" t="s">
         <v>10</v>
       </c>
       <c r="E71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F71" s="3">
         <v>33000000</v>
@@ -2065,13 +2062,13 @@
         <v>45832</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
       </c>
       <c r="E72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F72" s="3">
         <v>50000000</v>
@@ -2085,13 +2082,13 @@
         <v>45839</v>
       </c>
       <c r="C73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D73" t="s">
         <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F73" s="3">
         <v>13106000</v>
@@ -2105,13 +2102,13 @@
         <v>45839</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F74" s="3">
         <v>16894000</v>
@@ -2125,13 +2122,13 @@
         <v>45848</v>
       </c>
       <c r="C75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
       </c>
       <c r="E75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F75" s="3">
         <v>30000000</v>
@@ -2145,13 +2142,13 @@
         <v>45849</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D76" t="s">
         <v>10</v>
       </c>
       <c r="E76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F76" s="3">
         <v>30000000</v>
@@ -2165,13 +2162,13 @@
         <v>45860</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D77" t="s">
         <v>10</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F77" s="3">
         <v>25000000</v>
@@ -2185,13 +2182,13 @@
         <v>45867</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D78" t="s">
         <v>10</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F78" s="3">
         <v>25000000</v>
@@ -2205,13 +2202,13 @@
         <v>45867</v>
       </c>
       <c r="C79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D79" t="s">
         <v>10</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F79" s="3">
         <v>13750000</v>
@@ -2225,13 +2222,13 @@
         <v>45867</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D80" t="s">
         <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F80" s="3">
         <v>36200000</v>
@@ -2245,13 +2242,13 @@
         <v>45868</v>
       </c>
       <c r="C81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D81" t="s">
         <v>10</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F81" s="3">
         <v>40000000</v>
@@ -2265,13 +2262,13 @@
         <v>45870</v>
       </c>
       <c r="C82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F82" s="3">
         <v>50000000</v>
@@ -2285,13 +2282,13 @@
         <v>45877</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -2305,7 +2302,7 @@
         <v>45828</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
@@ -2325,13 +2322,13 @@
         <v>45832</v>
       </c>
       <c r="C85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D85" t="s">
         <v>10</v>
       </c>
       <c r="E85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F85">
         <v>100000000</v>
@@ -2345,13 +2342,13 @@
         <v>45834</v>
       </c>
       <c r="C86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D86" t="s">
         <v>10</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F86">
         <v>22000000</v>
@@ -2365,13 +2362,13 @@
         <v>45834</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F87">
         <v>20000000</v>
@@ -2385,13 +2382,13 @@
         <v>45834</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
       </c>
       <c r="E88" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F88">
         <v>4600000</v>
@@ -2405,13 +2402,13 @@
         <v>45835</v>
       </c>
       <c r="C89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
       </c>
       <c r="E89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F89">
         <v>13500000</v>
@@ -2425,13 +2422,13 @@
         <v>45835</v>
       </c>
       <c r="C90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D90" t="s">
         <v>10</v>
       </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F90">
         <v>6500000</v>
@@ -2445,13 +2442,13 @@
         <v>45841</v>
       </c>
       <c r="C91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D91" t="s">
         <v>10</v>
       </c>
       <c r="E91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F91">
         <v>22000000</v>
@@ -2465,13 +2462,13 @@
         <v>45841</v>
       </c>
       <c r="C92" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D92" t="s">
         <v>10</v>
       </c>
       <c r="E92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F92">
         <v>19000000</v>
@@ -2485,13 +2482,13 @@
         <v>45843</v>
       </c>
       <c r="C93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D93" t="s">
         <v>10</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F93">
         <v>50000000</v>
@@ -2505,13 +2502,13 @@
         <v>45848</v>
       </c>
       <c r="C94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D94" t="s">
         <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F94">
         <v>37000000</v>
@@ -2525,13 +2522,13 @@
         <v>45848</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D95" t="s">
         <v>10</v>
       </c>
       <c r="E95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F95">
         <v>19300000</v>
@@ -2545,13 +2542,13 @@
         <v>45861</v>
       </c>
       <c r="C96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D96" t="s">
         <v>10</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F96">
         <v>78000000</v>
@@ -2565,13 +2562,13 @@
         <v>45863</v>
       </c>
       <c r="C97" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D97" t="s">
         <v>10</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F97">
         <v>42000000</v>
@@ -2585,7 +2582,7 @@
         <v>45815</v>
       </c>
       <c r="C98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
@@ -2605,13 +2602,13 @@
         <v>45813</v>
       </c>
       <c r="C99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D99" t="s">
         <v>10</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F99">
         <v>44950000</v>
@@ -2625,13 +2622,13 @@
         <v>45814</v>
       </c>
       <c r="C100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D100" t="s">
         <v>10</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F100">
         <v>20000000</v>
@@ -2645,13 +2642,13 @@
         <v>45814</v>
       </c>
       <c r="C101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D101" t="s">
         <v>10</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F101">
         <v>50000000</v>
@@ -2665,13 +2662,13 @@
         <v>45815</v>
       </c>
       <c r="C102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D102" t="s">
         <v>10</v>
       </c>
       <c r="E102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F102">
         <v>9900000</v>
@@ -2685,13 +2682,13 @@
         <v>45816</v>
       </c>
       <c r="C103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D103" t="s">
         <v>10</v>
       </c>
       <c r="E103" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F103">
         <v>12000000</v>
@@ -2705,13 +2702,13 @@
         <v>45816</v>
       </c>
       <c r="C104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D104" t="s">
         <v>10</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F104">
         <v>6000000</v>
@@ -2725,13 +2722,13 @@
         <v>45816</v>
       </c>
       <c r="C105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
       </c>
       <c r="E105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F105">
         <v>2000000</v>
@@ -2745,13 +2742,13 @@
         <v>45816</v>
       </c>
       <c r="C106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D106" t="s">
         <v>10</v>
       </c>
       <c r="E106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F106">
         <v>100000</v>
@@ -2765,13 +2762,13 @@
         <v>45819</v>
       </c>
       <c r="C107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D107" t="s">
         <v>10</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F107">
         <v>50000000</v>
@@ -2785,13 +2782,13 @@
         <v>45821</v>
       </c>
       <c r="C108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D108" t="s">
         <v>10</v>
       </c>
       <c r="E108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F108">
         <v>50000000</v>
@@ -2805,13 +2802,13 @@
         <v>45822</v>
       </c>
       <c r="C109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
       </c>
       <c r="E109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F109">
         <v>15000000</v>
@@ -2825,13 +2822,13 @@
         <v>45822</v>
       </c>
       <c r="C110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D110" t="s">
         <v>10</v>
       </c>
       <c r="E110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F110">
         <v>10000000</v>
@@ -2845,13 +2842,13 @@
         <v>45826</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D111" t="s">
         <v>10</v>
       </c>
       <c r="E111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F111">
         <v>10000000</v>
@@ -2865,13 +2862,13 @@
         <v>45835</v>
       </c>
       <c r="C112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D112" t="s">
         <v>10</v>
       </c>
       <c r="E112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F112">
         <v>14140000</v>
@@ -2885,13 +2882,13 @@
         <v>45835</v>
       </c>
       <c r="C113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D113" t="s">
         <v>10</v>
       </c>
       <c r="E113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F113">
         <v>25860000</v>
@@ -2905,13 +2902,13 @@
         <v>45848</v>
       </c>
       <c r="C114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D114" t="s">
         <v>10</v>
       </c>
       <c r="E114" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F114">
         <v>10655000</v>
@@ -2925,13 +2922,13 @@
         <v>45842</v>
       </c>
       <c r="C115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D115" t="s">
         <v>10</v>
       </c>
       <c r="E115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F115">
         <v>27150000</v>
@@ -2945,13 +2942,13 @@
         <v>45842</v>
       </c>
       <c r="C116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D116" t="s">
         <v>10</v>
       </c>
       <c r="E116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F116">
         <v>2850000</v>
@@ -2965,13 +2962,13 @@
         <v>45842</v>
       </c>
       <c r="C117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D117" t="s">
         <v>10</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F117">
         <v>8000000</v>
@@ -2985,13 +2982,13 @@
         <v>45843</v>
       </c>
       <c r="C118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D118" t="s">
         <v>10</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F118">
         <v>5950000</v>
@@ -3005,7 +3002,7 @@
         <v>45843</v>
       </c>
       <c r="C119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D119" t="s">
         <v>7</v>
@@ -3025,13 +3022,13 @@
         <v>45846</v>
       </c>
       <c r="C120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D120" t="s">
         <v>10</v>
       </c>
       <c r="E120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F120">
         <v>15000000</v>
@@ -3045,13 +3042,13 @@
         <v>45847</v>
       </c>
       <c r="C121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D121" t="s">
         <v>10</v>
       </c>
       <c r="E121" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F121">
         <v>27087600</v>
@@ -3065,13 +3062,13 @@
         <v>45849</v>
       </c>
       <c r="C122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D122" t="s">
         <v>10</v>
       </c>
       <c r="E122" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F122">
         <v>25000000</v>
@@ -3085,13 +3082,13 @@
         <v>45849</v>
       </c>
       <c r="C123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D123" t="s">
         <v>10</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F123">
         <v>40000000</v>
@@ -3105,7 +3102,7 @@
         <v>45850</v>
       </c>
       <c r="C124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D124" t="s">
         <v>7</v>
@@ -3125,13 +3122,13 @@
         <v>45863</v>
       </c>
       <c r="C125" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D125" t="s">
         <v>10</v>
       </c>
       <c r="E125" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F125">
         <v>20000000</v>
@@ -3145,13 +3142,13 @@
         <v>45867</v>
       </c>
       <c r="C126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D126" t="s">
         <v>10</v>
       </c>
       <c r="E126" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F126">
         <v>2600000</v>
@@ -3165,13 +3162,13 @@
         <v>45863</v>
       </c>
       <c r="C127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D127" t="s">
         <v>10</v>
       </c>
       <c r="E127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F127">
         <v>25000000</v>
@@ -3185,13 +3182,13 @@
         <v>45867</v>
       </c>
       <c r="C128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D128" t="s">
         <v>10</v>
       </c>
       <c r="E128" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F128">
         <v>400000</v>
@@ -3205,13 +3202,13 @@
         <v>45869</v>
       </c>
       <c r="C129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D129" t="s">
         <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F129">
         <v>25000000</v>
@@ -3225,13 +3222,13 @@
         <v>45870</v>
       </c>
       <c r="C130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D130" t="s">
         <v>10</v>
       </c>
       <c r="E130" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F130">
         <v>17922000</v>
@@ -3245,13 +3242,13 @@
         <v>45875</v>
       </c>
       <c r="C131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D131" t="s">
         <v>10</v>
       </c>
       <c r="E131" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F131">
         <v>22600000</v>
@@ -3265,7 +3262,7 @@
         <v>45869</v>
       </c>
       <c r="C132" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D132" t="s">
         <v>7</v>
@@ -3285,13 +3282,13 @@
         <v>45869</v>
       </c>
       <c r="C133" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D133" t="s">
         <v>10</v>
       </c>
       <c r="E133" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F133">
         <v>15000000</v>
@@ -3305,13 +3302,13 @@
         <v>45869</v>
       </c>
       <c r="C134" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D134" t="s">
         <v>10</v>
       </c>
       <c r="E134" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F134">
         <v>5000000</v>
@@ -3325,13 +3322,13 @@
         <v>45869</v>
       </c>
       <c r="C135" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D135" t="s">
         <v>10</v>
       </c>
       <c r="E135" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F135">
         <v>40000000</v>
@@ -3345,13 +3342,13 @@
         <v>45869</v>
       </c>
       <c r="C136" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D136" t="s">
         <v>10</v>
       </c>
       <c r="E136" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F136">
         <v>23000000</v>
@@ -3365,13 +3362,13 @@
         <v>45870</v>
       </c>
       <c r="C137" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D137" t="s">
         <v>10</v>
       </c>
       <c r="E137" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F137">
         <v>1000000</v>
@@ -3385,7 +3382,7 @@
         <v>45870</v>
       </c>
       <c r="C138" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D138" t="s">
         <v>7</v>
@@ -3405,7 +3402,7 @@
         <v>45872</v>
       </c>
       <c r="C139" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D139" t="s">
         <v>7</v>
@@ -3425,13 +3422,13 @@
         <v>45873</v>
       </c>
       <c r="C140" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D140" t="s">
         <v>10</v>
       </c>
       <c r="E140" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F140">
         <v>15386000</v>
@@ -3445,13 +3442,13 @@
         <v>45873</v>
       </c>
       <c r="C141" t="s">
+        <v>17</v>
+      </c>
+      <c r="D141" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" t="s">
         <v>18</v>
-      </c>
-      <c r="D141" t="s">
-        <v>10</v>
-      </c>
-      <c r="E141" t="s">
-        <v>19</v>
       </c>
       <c r="F141">
         <v>2000000</v>
@@ -3465,13 +3462,13 @@
         <v>45877</v>
       </c>
       <c r="C142" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D142" t="s">
         <v>10</v>
       </c>
       <c r="E142" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F142">
         <v>38000000</v>
@@ -3485,13 +3482,13 @@
         <v>45875</v>
       </c>
       <c r="C143" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D143" t="s">
         <v>10</v>
       </c>
       <c r="E143" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F143">
         <v>22000000</v>
@@ -3505,13 +3502,13 @@
         <v>45875</v>
       </c>
       <c r="C144" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D144" t="s">
         <v>10</v>
       </c>
       <c r="E144" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F144">
         <v>22000000</v>
@@ -3525,13 +3522,13 @@
         <v>45875</v>
       </c>
       <c r="C145" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D145" t="s">
         <v>10</v>
       </c>
       <c r="E145" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F145">
         <v>20000000</v>
@@ -3545,13 +3542,13 @@
         <v>45875</v>
       </c>
       <c r="C146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D146" t="s">
         <v>10</v>
       </c>
       <c r="E146" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F146">
         <v>36640500</v>
@@ -3565,13 +3562,13 @@
         <v>45877</v>
       </c>
       <c r="C147" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D147" t="s">
         <v>10</v>
       </c>
       <c r="E147" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F147">
         <v>20000000</v>
@@ -3585,7 +3582,7 @@
         <v>45860</v>
       </c>
       <c r="C148" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D148" t="s">
         <v>7</v>
@@ -3610,8 +3607,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3630,7 +3627,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>21</v>
@@ -3661,7 +3658,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
         <v>357288650</v>
@@ -3678,7 +3675,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>591739250</v>
@@ -3695,7 +3692,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
         <v>388594900</v>
@@ -3712,7 +3709,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3">
         <v>648442750</v>
@@ -3729,7 +3726,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3">
         <v>204357400</v>
@@ -3753,7 +3750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3785,7 +3784,7 @@
         <v>45880</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -3807,7 +3806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3819,7 +3820,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>21</v>
@@ -3833,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>50000000</v>

</xml_diff>